<commit_message>
Finalised V1 for production
Finalised V1 for production. added hot symbol, moved mounting holes to
better location, fixed remaining drc error, and tiedied up silkscreen
</commit_message>
<xml_diff>
--- a/Docs/OSBMS MicroMaster BOM.xlsx
+++ b/Docs/OSBMS MicroMaster BOM.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>